<commit_message>
Updated and cleaned dataset
</commit_message>
<xml_diff>
--- a/Hong Kong Covariates.xlsx
+++ b/Hong Kong Covariates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ornellanoubissiewafo/Documents/GitHub/Spatial-Epidemiology---Cov-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC90578C-E2FE-9744-A594-74A2502784D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F6DE2779-267F-124E-A63B-E279009C3A12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="1360" windowWidth="30420" windowHeight="13360" xr2:uid="{492455BD-E665-5E4C-88AE-22B51FC8041B}"/>
   </bookViews>
@@ -486,7 +486,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -495,9 +495,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -511,7 +508,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="170" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -520,7 +516,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -529,10 +528,15 @@
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -852,77 +856,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2153849-5DC7-E344-9210-D8828C138895}">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="O18" sqref="O18"/>
+      <selection pane="topRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="13"/>
-    <col min="4" max="4" width="13.5" style="13" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="13" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="22" customWidth="1"/>
-    <col min="7" max="8" width="10.83203125" style="13"/>
-    <col min="9" max="9" width="13.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" style="25"/>
-    <col min="15" max="16384" width="10.83203125" style="13"/>
+    <col min="1" max="1" width="9.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="21"/>
+    <col min="4" max="4" width="13.5" style="11" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="11" customWidth="1"/>
+    <col min="6" max="6" width="14.5" style="21" customWidth="1"/>
+    <col min="7" max="8" width="10.83203125" style="11"/>
+    <col min="9" max="9" width="13.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" style="23"/>
+    <col min="15" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="11" customFormat="1">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:16" s="10" customFormat="1">
+      <c r="A1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="10" t="s">
         <v>95</v>
       </c>
     </row>
@@ -933,51 +937,51 @@
       <c r="B2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="25">
         <v>107700</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="25">
         <v>133900</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="25">
         <v>241500</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="20">
         <f>E2/7306700*100</f>
         <v>3.3051856515253122</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="26">
         <v>12.44</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="21">
         <f>E2/G2</f>
         <v>19413.183279742767</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="25">
         <v>141800</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2" s="17">
         <f>100*I2/E2</f>
         <v>58.716356107660452</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="25">
         <v>75100</v>
       </c>
-      <c r="L2" s="25">
+      <c r="L2" s="18">
         <f>100*K2/D2</f>
         <v>56.086631814787154</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="25">
         <v>66700</v>
       </c>
-      <c r="N2" s="25">
+      <c r="N2" s="18">
         <f>100*M2/C2</f>
         <v>61.931290622098423</v>
       </c>
-      <c r="O2" s="13">
+      <c r="O2" s="21">
         <v>2</v>
       </c>
-      <c r="P2" s="13">
+      <c r="P2" s="21">
         <v>535</v>
       </c>
     </row>
@@ -988,51 +992,51 @@
       <c r="B3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="25">
         <v>78300</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="25">
         <v>101100</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="25">
         <v>179400</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="20">
         <f t="shared" ref="F3:F19" si="0">E3/7306700*100</f>
         <v>2.4552807697045176</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="26">
         <v>9.83</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="21">
         <f>E3/G3</f>
         <v>18250.254323499492</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="25">
         <v>104400</v>
       </c>
-      <c r="J3" s="24">
+      <c r="J3" s="17">
         <f t="shared" ref="J3:J4" si="1">100*I3/E3</f>
         <v>58.19397993311037</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="25">
         <v>55500</v>
       </c>
-      <c r="L3" s="25">
+      <c r="L3" s="18">
         <f t="shared" ref="L3:L19" si="2">100*K3/D3</f>
         <v>54.896142433234424</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="25">
         <v>48900</v>
       </c>
-      <c r="N3" s="25">
+      <c r="N3" s="18">
         <f t="shared" ref="N3:N19" si="3">100*M3/C3</f>
         <v>62.452107279693486</v>
       </c>
-      <c r="O3" s="13">
+      <c r="O3" s="21">
         <v>2</v>
       </c>
-      <c r="P3" s="19">
+      <c r="P3" s="27">
         <v>886</v>
       </c>
     </row>
@@ -1043,51 +1047,51 @@
       <c r="B4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="25">
         <v>244800</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="25">
         <v>301600</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="25">
         <v>546400</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="20">
         <f t="shared" si="0"/>
         <v>7.4780680745069592</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="26">
         <v>18.559999999999999</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="21">
         <f>E4/G4</f>
         <v>29439.655172413793</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="25">
         <v>297700</v>
       </c>
-      <c r="J4" s="24">
+      <c r="J4" s="17">
         <f t="shared" si="1"/>
         <v>54.483894582723281</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="25">
         <v>154200</v>
       </c>
-      <c r="L4" s="25">
+      <c r="L4" s="18">
         <f t="shared" si="2"/>
         <v>51.127320954907162</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="25">
         <v>143500</v>
       </c>
-      <c r="N4" s="25">
+      <c r="N4" s="18">
         <f t="shared" si="3"/>
         <v>58.619281045751634</v>
       </c>
-      <c r="O4" s="13">
+      <c r="O4" s="21">
         <v>1</v>
       </c>
-      <c r="P4" s="19">
+      <c r="P4" s="27">
         <v>1739</v>
       </c>
     </row>
@@ -1098,51 +1102,51 @@
       <c r="B5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="25">
         <v>118500</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="25">
         <v>145400</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="25">
         <v>263900</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="20">
         <f t="shared" si="0"/>
         <v>3.611753596014617</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="26">
         <v>38.85</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="21">
         <f>E5/G5</f>
         <v>6792.7927927927922</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="25">
         <v>147800</v>
       </c>
-      <c r="J5" s="24">
+      <c r="J5" s="17">
         <f>100*I5/E5</f>
         <v>56.00606290261463</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="25">
         <v>76800</v>
       </c>
-      <c r="L5" s="25">
+      <c r="L5" s="18">
         <f t="shared" si="2"/>
         <v>52.81980742778542</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="25">
         <v>71000</v>
       </c>
-      <c r="N5" s="25">
+      <c r="N5" s="18">
         <f t="shared" si="3"/>
         <v>59.915611814345993</v>
       </c>
-      <c r="O5" s="13">
+      <c r="O5" s="21">
         <v>7</v>
       </c>
-      <c r="P5" s="13">
+      <c r="P5" s="21">
         <v>3009</v>
       </c>
     </row>
@@ -1153,51 +1157,51 @@
       <c r="B6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="25">
         <v>153800</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="25">
         <v>179800</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="25">
         <v>333600</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="20">
         <f t="shared" si="0"/>
         <v>4.5656726018585685</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="26">
         <v>6.99</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="21">
         <f>E6/G6</f>
         <v>47725.321888412014</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="25">
         <v>186800</v>
       </c>
-      <c r="J6" s="24">
+      <c r="J6" s="17">
         <f t="shared" ref="J6:J19" si="4">100*I6/E6</f>
         <v>55.995203836930457</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="25">
         <v>92900</v>
       </c>
-      <c r="L6" s="25">
+      <c r="L6" s="18">
         <f t="shared" si="2"/>
         <v>51.66852057842047</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="25">
         <v>93800</v>
       </c>
-      <c r="N6" s="25">
+      <c r="N6" s="18">
         <f t="shared" si="3"/>
         <v>60.988296488946681</v>
       </c>
-      <c r="O6" s="13">
+      <c r="O6" s="21">
         <v>1</v>
       </c>
-      <c r="P6" s="19">
+      <c r="P6" s="27">
         <v>1186</v>
       </c>
     </row>
@@ -1208,51 +1212,51 @@
       <c r="B7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="25">
         <v>185000</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="25">
         <v>215600</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="25">
         <v>400500</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="20">
         <f t="shared" si="0"/>
         <v>5.4812706146413568</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="26">
         <v>9.35</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="21">
         <f>E7/G7</f>
         <v>42834.224598930487</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="25">
         <v>214600</v>
       </c>
-      <c r="J7" s="24">
+      <c r="J7" s="17">
         <f t="shared" si="4"/>
         <v>53.583021223470659</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="25">
         <v>106100</v>
       </c>
-      <c r="L7" s="25">
+      <c r="L7" s="18">
         <f t="shared" si="2"/>
         <v>49.211502782931355</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="25">
         <v>108500</v>
       </c>
-      <c r="N7" s="25">
+      <c r="N7" s="18">
         <f t="shared" si="3"/>
         <v>58.648648648648646</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O7" s="21">
         <v>1</v>
       </c>
-      <c r="P7" s="19">
+      <c r="P7" s="27">
         <v>1206</v>
       </c>
     </row>
@@ -1263,51 +1267,51 @@
       <c r="B8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="25">
         <v>186100</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="25">
         <v>225800</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="25">
         <v>411900</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="20">
         <f t="shared" si="0"/>
         <v>5.6372918006760919</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="26">
         <v>10.02</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="21">
         <f>E8/G8</f>
         <v>41107.784431137727</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="25">
         <v>222400</v>
       </c>
-      <c r="J8" s="24">
+      <c r="J8" s="17">
         <f t="shared" si="4"/>
         <v>53.993687788298132</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="25">
         <v>114600</v>
       </c>
-      <c r="L8" s="25">
+      <c r="L8" s="18">
         <f t="shared" si="2"/>
         <v>50.752878653675822</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="25">
         <v>107800</v>
       </c>
-      <c r="N8" s="25">
+      <c r="N8" s="18">
         <f t="shared" si="3"/>
         <v>57.925846319183236</v>
       </c>
-      <c r="O8" s="13">
+      <c r="O8" s="21">
         <v>4</v>
       </c>
-      <c r="P8" s="13">
+      <c r="P8" s="21">
         <v>3405</v>
       </c>
     </row>
@@ -1318,51 +1322,51 @@
       <c r="B9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="25">
         <v>195800</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="25">
         <v>224800</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="25">
         <v>420600</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="20">
         <f t="shared" si="0"/>
         <v>5.7563606005447054</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="26">
         <v>9.3000000000000007</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="21">
         <f>E9/G9</f>
         <v>45225.806451612902</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="25">
         <v>221100</v>
       </c>
-      <c r="J9" s="24">
+      <c r="J9" s="17">
         <f t="shared" si="4"/>
         <v>52.567760342368047</v>
       </c>
-      <c r="K9" s="5">
+      <c r="K9" s="25">
         <v>106700</v>
       </c>
-      <c r="L9" s="25">
+      <c r="L9" s="18">
         <f t="shared" si="2"/>
         <v>47.464412811387902</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="25">
         <v>114400</v>
       </c>
-      <c r="N9" s="25">
+      <c r="N9" s="18">
         <f t="shared" si="3"/>
         <v>58.426966292134829</v>
       </c>
-      <c r="O9" s="13">
+      <c r="O9" s="21">
         <v>3</v>
       </c>
-      <c r="P9" s="19">
+      <c r="P9" s="27">
         <v>1091</v>
       </c>
     </row>
@@ -1373,51 +1377,51 @@
       <c r="B10" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="25">
         <v>308800</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="25">
         <v>355300</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="25">
         <v>664100</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="20">
         <f t="shared" si="0"/>
         <v>9.0889183899708481</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="26">
         <v>11.27</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="21">
         <f>E10/G10</f>
         <v>58926.353149955634</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="25">
         <v>346500</v>
       </c>
-      <c r="J10" s="24">
+      <c r="J10" s="17">
         <f t="shared" si="4"/>
         <v>52.175877126938715</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K10" s="25">
         <v>167800</v>
       </c>
-      <c r="L10" s="25">
+      <c r="L10" s="18">
         <f t="shared" si="2"/>
         <v>47.227694905713484</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="25">
         <v>178700</v>
       </c>
-      <c r="N10" s="25">
+      <c r="N10" s="18">
         <f t="shared" si="3"/>
         <v>57.869170984455955</v>
       </c>
-      <c r="O10" s="13">
+      <c r="O10" s="21">
         <v>1</v>
       </c>
-      <c r="P10" s="19">
+      <c r="P10" s="27">
         <v>1415</v>
       </c>
     </row>
@@ -1428,51 +1432,51 @@
       <c r="B11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="25">
         <v>237200</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="25">
         <v>270400</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="25">
         <v>507700</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="20">
         <f t="shared" si="0"/>
         <v>6.9484172061258844</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="26">
         <v>23.34</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="21">
         <f>E11/G11</f>
         <v>21752.356469580121</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="25">
         <v>269000</v>
       </c>
-      <c r="J11" s="24">
+      <c r="J11" s="17">
         <f t="shared" si="4"/>
         <v>52.984045696277327</v>
       </c>
-      <c r="K11" s="5">
+      <c r="K11" s="25">
         <v>129700</v>
       </c>
-      <c r="L11" s="25">
+      <c r="L11" s="18">
         <f t="shared" si="2"/>
         <v>47.965976331360949</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="25">
         <v>139200</v>
       </c>
-      <c r="N11" s="25">
+      <c r="N11" s="18">
         <f t="shared" si="3"/>
         <v>58.684654300168631</v>
       </c>
-      <c r="O11" s="13">
+      <c r="O11" s="21">
         <v>2</v>
       </c>
-      <c r="P11" s="19">
+      <c r="P11" s="27">
         <v>2653</v>
       </c>
     </row>
@@ -1483,51 +1487,51 @@
       <c r="B12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="25">
         <v>144600</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="25">
         <v>169000</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="25">
         <v>313600</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="20">
         <f>E12/7306700*100</f>
         <v>4.291951222850261</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="26">
         <v>61.71</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="21">
         <f>E12/G12</f>
         <v>5081.8343866472205</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="25">
         <v>175900</v>
       </c>
-      <c r="J12" s="24">
+      <c r="J12" s="17">
         <f t="shared" si="4"/>
         <v>56.090561224489797</v>
       </c>
-      <c r="K12" s="5">
+      <c r="K12" s="25">
         <v>86300</v>
       </c>
-      <c r="L12" s="25">
+      <c r="L12" s="18">
         <f t="shared" si="2"/>
         <v>51.065088757396452</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="25">
         <v>89600</v>
       </c>
-      <c r="N12" s="25">
+      <c r="N12" s="18">
         <f t="shared" si="3"/>
         <v>61.964038727524205</v>
       </c>
-      <c r="O12" s="13">
+      <c r="O12" s="21">
         <v>1</v>
       </c>
-      <c r="P12" s="13">
+      <c r="P12" s="21">
         <v>800</v>
       </c>
     </row>
@@ -1538,51 +1542,51 @@
       <c r="B13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="25">
         <v>224300</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="25">
         <v>256200</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="25">
         <v>480500</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="20">
         <f t="shared" si="0"/>
         <v>6.5761561306745859</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="26">
         <v>82.89</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="21">
         <f>E13/G13</f>
         <v>5796.8391844613343</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="25">
         <v>261200</v>
       </c>
-      <c r="J13" s="24">
+      <c r="J13" s="17">
         <f t="shared" si="4"/>
         <v>54.360041623309051</v>
       </c>
-      <c r="K13" s="5">
+      <c r="K13" s="25">
         <v>123300</v>
       </c>
-      <c r="L13" s="25">
+      <c r="L13" s="18">
         <f t="shared" si="2"/>
         <v>48.12646370023419</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="25">
         <v>137900</v>
       </c>
-      <c r="N13" s="25">
+      <c r="N13" s="18">
         <f t="shared" si="3"/>
         <v>61.480160499331255</v>
       </c>
-      <c r="O13" s="13">
+      <c r="O13" s="21">
         <v>3</v>
       </c>
-      <c r="P13" s="19">
+      <c r="P13" s="27">
         <v>3591</v>
       </c>
     </row>
@@ -1593,51 +1597,51 @@
       <c r="B14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="25">
         <v>290200</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="25">
         <v>334800</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="25">
         <v>625000</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="20">
         <f t="shared" si="0"/>
         <v>8.5537930940096079</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="26">
         <v>138.46</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="21">
         <f>E14/G14</f>
         <v>4513.9390437671527</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="25">
         <v>329600</v>
       </c>
-      <c r="J14" s="24">
+      <c r="J14" s="17">
         <f t="shared" si="4"/>
         <v>52.735999999999997</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14" s="25">
         <v>158000</v>
       </c>
-      <c r="L14" s="25">
+      <c r="L14" s="18">
         <f t="shared" si="2"/>
         <v>47.192353643966548</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14" s="25">
         <v>171600</v>
       </c>
-      <c r="N14" s="25">
+      <c r="N14" s="18">
         <f t="shared" si="3"/>
         <v>59.131633356305997</v>
       </c>
-      <c r="O14" s="13">
+      <c r="O14" s="21">
         <v>2</v>
       </c>
-      <c r="P14" s="19">
+      <c r="P14" s="27">
         <v>1095</v>
       </c>
     </row>
@@ -1648,51 +1652,51 @@
       <c r="B15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="25">
         <v>146900</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="25">
         <v>165900</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="25">
         <v>312700</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="20">
         <f t="shared" si="0"/>
         <v>4.2796337607948871</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="26">
         <v>136.61000000000001</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="21">
         <f>E15/G15</f>
         <v>2288.9978771685819</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="25">
         <v>158500</v>
       </c>
-      <c r="J15" s="24">
+      <c r="J15" s="17">
         <f t="shared" si="4"/>
         <v>50.687559961624558</v>
       </c>
-      <c r="K15" s="5">
+      <c r="K15" s="25">
         <v>72900</v>
       </c>
-      <c r="L15" s="25">
+      <c r="L15" s="18">
         <f t="shared" si="2"/>
         <v>43.942133815551536</v>
       </c>
-      <c r="M15" s="5">
+      <c r="M15" s="25">
         <v>85600</v>
       </c>
-      <c r="N15" s="25">
+      <c r="N15" s="18">
         <f t="shared" si="3"/>
         <v>58.270932607215791</v>
       </c>
-      <c r="O15" s="13">
+      <c r="O15" s="21">
         <v>1</v>
       </c>
-      <c r="P15" s="13">
+      <c r="P15" s="21">
         <v>600</v>
       </c>
     </row>
@@ -1703,51 +1707,51 @@
       <c r="B16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="25">
         <v>139400</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="25">
         <v>164200</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="25">
         <v>303700</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="20">
         <f t="shared" si="0"/>
         <v>4.1564591402411484</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="26">
         <v>136.15</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="21">
         <f>E16/G16</f>
         <v>2230.6279838413516</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="25">
         <v>161900</v>
       </c>
-      <c r="J16" s="24">
+      <c r="J16" s="17">
         <f t="shared" si="4"/>
         <v>53.309186697398751</v>
       </c>
-      <c r="K16" s="5">
+      <c r="K16" s="25">
         <v>78600</v>
       </c>
-      <c r="L16" s="25">
+      <c r="L16" s="18">
         <f t="shared" si="2"/>
         <v>47.868453105968328</v>
       </c>
-      <c r="M16" s="5">
+      <c r="M16" s="25">
         <v>83300</v>
       </c>
-      <c r="N16" s="25">
+      <c r="N16" s="18">
         <f t="shared" si="3"/>
         <v>59.756097560975611</v>
       </c>
-      <c r="O16" s="13">
+      <c r="O16" s="21">
         <v>2</v>
       </c>
-      <c r="P16" s="19">
+      <c r="P16" s="27">
         <v>1555</v>
       </c>
     </row>
@@ -1758,51 +1762,51 @@
       <c r="B17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="25">
         <v>309800</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="25">
         <v>367800</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="25">
         <v>677600</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="20">
         <f t="shared" si="0"/>
         <v>9.2736803208014553</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="26">
         <v>68.709999999999994</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="21">
         <f>E17/G17</f>
         <v>9861.7377383204785</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I17" s="25">
         <v>360400</v>
       </c>
-      <c r="J17" s="24">
+      <c r="J17" s="17">
         <f t="shared" si="4"/>
         <v>53.187721369539553</v>
       </c>
-      <c r="K17" s="5">
+      <c r="K17" s="25">
         <v>178000</v>
       </c>
-      <c r="L17" s="25">
+      <c r="L17" s="18">
         <f t="shared" si="2"/>
         <v>48.395867319195212</v>
       </c>
-      <c r="M17" s="5">
+      <c r="M17" s="25">
         <v>182400</v>
       </c>
-      <c r="N17" s="25">
+      <c r="N17" s="18">
         <f t="shared" si="3"/>
         <v>58.876694641704326</v>
       </c>
-      <c r="O17" s="13">
+      <c r="O17" s="21">
         <v>4</v>
       </c>
-      <c r="P17" s="19">
+      <c r="P17" s="27">
         <v>2589</v>
       </c>
     </row>
@@ -1813,51 +1817,51 @@
       <c r="B18" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="25">
         <v>211200</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="25">
         <v>252600</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="25">
         <v>463700</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="20">
         <f t="shared" si="0"/>
         <v>6.3462301723076084</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="26">
         <v>129.65</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="21">
         <f>E18/G18</f>
         <v>3576.5522560740455</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18" s="25">
         <v>259000</v>
       </c>
-      <c r="J18" s="24">
+      <c r="J18" s="17">
         <f t="shared" si="4"/>
         <v>55.855078714686222</v>
       </c>
-      <c r="K18" s="5">
+      <c r="K18" s="25">
         <v>130900</v>
       </c>
-      <c r="L18" s="25">
+      <c r="L18" s="18">
         <f t="shared" si="2"/>
         <v>51.821060965954075</v>
       </c>
-      <c r="M18" s="5">
+      <c r="M18" s="25">
         <v>128100</v>
       </c>
-      <c r="N18" s="25">
+      <c r="N18" s="18">
         <f t="shared" si="3"/>
         <v>60.653409090909093</v>
       </c>
-      <c r="O18" s="13">
+      <c r="O18" s="21">
         <v>2</v>
       </c>
-      <c r="P18" s="19">
+      <c r="P18" s="27">
         <v>1128</v>
       </c>
     </row>
@@ -1868,59 +1872,56 @@
       <c r="B19" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="25">
         <v>71700</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="25">
         <v>88600</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="25">
         <v>160300</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="20">
         <f t="shared" si="0"/>
         <v>2.193876852751584</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="26">
         <v>175.12</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="21">
         <f>E19/G19</f>
         <v>915.37231612608491</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19" s="25">
         <v>88100</v>
       </c>
-      <c r="J19" s="24">
+      <c r="J19" s="17">
         <f t="shared" si="4"/>
         <v>54.959451029320022</v>
       </c>
-      <c r="K19" s="5">
+      <c r="K19" s="25">
         <v>44900</v>
       </c>
-      <c r="L19" s="25">
+      <c r="L19" s="18">
         <f t="shared" si="2"/>
         <v>50.677200902934537</v>
       </c>
-      <c r="M19" s="5">
+      <c r="M19" s="25">
         <v>43100</v>
       </c>
-      <c r="N19" s="25">
+      <c r="N19" s="18">
         <f t="shared" si="3"/>
         <v>60.111576011157602</v>
       </c>
-      <c r="O19" s="13">
+      <c r="O19" s="21">
         <v>2</v>
       </c>
-      <c r="P19" s="19">
+      <c r="P19" s="27">
         <v>247</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
-      <c r="C20" s="14"/>
-    </row>
     <row r="25" spans="1:16">
-      <c r="D25" s="14"/>
+      <c r="D25" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:P19" xr:uid="{DAA0BDA6-480F-4344-8734-EA5FBDE524D1}"/>
@@ -1943,20 +1944,20 @@
     <col min="3" max="3" width="60" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:5" s="5" customFormat="1">
+      <c r="A1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1967,7 +1968,7 @@
       <c r="B2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D2">
@@ -2054,7 +2055,7 @@
       <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D8">
@@ -2068,7 +2069,7 @@
       <c r="B9" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D9">
@@ -2082,7 +2083,7 @@
       <c r="B10" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>72</v>
       </c>
       <c r="D10">
@@ -2096,7 +2097,7 @@
       <c r="B11" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D11">
@@ -2110,7 +2111,7 @@
       <c r="B12" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>73</v>
       </c>
       <c r="D12">
@@ -2124,7 +2125,7 @@
       <c r="B13" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D13">
@@ -2132,7 +2133,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="15" t="s">
         <v>32</v>
       </c>
       <c r="B14" t="s">
@@ -2286,7 +2287,7 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="16" t="s">
         <v>45</v>
       </c>
       <c r="B25" t="s">

</xml_diff>